<commit_message>
lots of results explorations
</commit_message>
<xml_diff>
--- a/notebooks/data/etiology.xlsx
+++ b/notebooks/data/etiology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louis/git/Tinnitus-n-Sleep/notebooks/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeta\Documents\acou_sommeil_HD_ENS\Tinnitus-n-Sleep\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3851529E-841B-BD4D-AA13-F0D1CBA601AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985E213A-1AA6-4BF7-B8DE-B35EB7F72BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52800" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{F5BF53D5-4C89-465E-97CD-524ECB77F3A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F5BF53D5-4C89-465E-97CD-524ECB77F3A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="395">
   <si>
     <t>Homme</t>
   </si>
@@ -1216,7 +1216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1624,18 +1624,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E847EA8-6EE2-42D7-BAB1-4873AF742906}">
   <dimension ref="A1:FX76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EA1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="topRight" activeCell="EI33" sqref="EI33"/>
+      <selection pane="topRight" activeCell="CN30" sqref="CN30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="59" max="59" width="10.83203125" style="5"/>
+    <col min="59" max="59" width="10.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:180">
       <c r="A1" t="s">
         <v>300</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:180">
       <c r="A2" s="3" t="s">
         <v>302</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>44033.817847222221</v>
       </c>
     </row>
-    <row r="3" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:180">
       <c r="A3" s="3" t="s">
         <v>314</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>43846.486921296295</v>
       </c>
     </row>
-    <row r="4" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:180">
       <c r="A4" s="3" t="s">
         <v>305</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>44029.723680555559</v>
       </c>
     </row>
-    <row r="5" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:180">
       <c r="A5" s="3" t="s">
         <v>307</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>43970.600405092591</v>
       </c>
     </row>
-    <row r="6" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:180">
       <c r="A6" s="3" t="s">
         <v>306</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>43887.003888888888</v>
       </c>
     </row>
-    <row r="7" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:180">
       <c r="A7" s="3" t="s">
         <v>304</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>44029.823275462964</v>
       </c>
     </row>
-    <row r="8" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:180">
       <c r="A8" s="3" t="s">
         <v>303</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>44036.38894675926</v>
       </c>
     </row>
-    <row r="9" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:180">
       <c r="A9" s="3" t="s">
         <v>386</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>44068.474166666667</v>
       </c>
     </row>
-    <row r="10" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:180">
       <c r="A10" s="4" t="s">
         <v>311</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>43729.039687500001</v>
       </c>
     </row>
-    <row r="11" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:180">
       <c r="A11" s="4" t="s">
         <v>308</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>43718.933912037035</v>
       </c>
     </row>
-    <row r="12" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:180">
       <c r="A12" s="4" t="s">
         <v>309</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>43720.592141203706</v>
       </c>
     </row>
-    <row r="13" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:180">
       <c r="A13" s="4" t="s">
         <v>301</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>44053.677824074075</v>
       </c>
     </row>
-    <row r="14" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:180">
       <c r="A14" s="4" t="s">
         <v>312</v>
       </c>
@@ -6616,7 +6616,7 @@
         <v>43756.492511574077</v>
       </c>
     </row>
-    <row r="15" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:180">
       <c r="A15" s="4" t="s">
         <v>313</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>43765.896203703705</v>
       </c>
     </row>
-    <row r="16" spans="1:180" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:180">
       <c r="A16" s="4" t="s">
         <v>310</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>43723.830752314818</v>
       </c>
     </row>
-    <row r="17" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:180" s="5" customFormat="1">
       <c r="A17" s="5" t="s">
         <v>320</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>43717.625</v>
       </c>
     </row>
-    <row r="18" spans="1:180" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:180" s="8" customFormat="1">
       <c r="A18" s="8" t="s">
         <v>327</v>
       </c>
@@ -7929,7 +7929,7 @@
         <v>43717.869444444441</v>
       </c>
     </row>
-    <row r="19" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:180" s="5" customFormat="1">
       <c r="A19" s="5" t="s">
         <v>332</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>43717.697222222225</v>
       </c>
     </row>
-    <row r="20" spans="1:180" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:180" s="11" customFormat="1">
       <c r="A20" s="11" t="s">
         <v>335</v>
       </c>
@@ -8561,7 +8561,7 @@
         <v>43717.730555555558</v>
       </c>
     </row>
-    <row r="21" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:180" s="5" customFormat="1">
       <c r="A21" s="5" t="s">
         <v>338</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>43719.534722222219</v>
       </c>
     </row>
-    <row r="22" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:180" s="5" customFormat="1">
       <c r="A22" s="5" t="s">
         <v>342</v>
       </c>
@@ -9210,7 +9210,7 @@
         <v>43719.566666666666</v>
       </c>
     </row>
-    <row r="23" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:180" s="5" customFormat="1">
       <c r="A23" s="5" t="s">
         <v>346</v>
       </c>
@@ -9542,7 +9542,7 @@
         <v>43738.599305555559</v>
       </c>
     </row>
-    <row r="24" spans="1:180" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:180" s="11" customFormat="1">
       <c r="A24" s="11" t="s">
         <v>351</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>43745.912499999999</v>
       </c>
     </row>
-    <row r="25" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:180" s="5" customFormat="1">
       <c r="A25" s="5" t="s">
         <v>354</v>
       </c>
@@ -10189,7 +10189,7 @@
         <v>43753.380555555559</v>
       </c>
     </row>
-    <row r="26" spans="1:180" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:180" s="14" customFormat="1">
       <c r="A26" s="14" t="s">
         <v>357</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>43758.751388888886</v>
       </c>
     </row>
-    <row r="27" spans="1:180" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:180" s="11" customFormat="1">
       <c r="A27" s="11" t="s">
         <v>361</v>
       </c>
@@ -10733,7 +10733,7 @@
         <v>43763.501388888886</v>
       </c>
     </row>
-    <row r="28" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:180" s="5" customFormat="1">
       <c r="A28" s="5" t="s">
         <v>365</v>
       </c>
@@ -11077,7 +11077,7 @@
         <v>43769.868750000001</v>
       </c>
     </row>
-    <row r="29" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:180" s="5" customFormat="1">
       <c r="A29" s="5" t="s">
         <v>369</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>43770.369444444441</v>
       </c>
     </row>
-    <row r="30" spans="1:180" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:180" s="5" customFormat="1" ht="15.5">
       <c r="A30" s="17" t="s">
         <v>387</v>
       </c>
@@ -11425,9 +11425,15 @@
       <c r="BZ30" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="CB30" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="CD30" t="s">
         <v>13</v>
       </c>
+      <c r="CF30" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="CI30" s="5" t="s">
         <v>13</v>
       </c>
@@ -11435,7 +11441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:180" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:180" s="5" customFormat="1" ht="15.5">
       <c r="A31" s="17" t="s">
         <v>388</v>
       </c>
@@ -11448,6 +11454,9 @@
       <c r="D31" s="18">
         <v>50</v>
       </c>
+      <c r="AF31" s="5">
+        <v>1</v>
+      </c>
       <c r="BN31" t="s">
         <v>31</v>
       </c>
@@ -11460,17 +11469,26 @@
       <c r="BZ31" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="CB31" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="CD31" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="CF31" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="CI31" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="DF31" s="5">
+        <v>1</v>
+      </c>
       <c r="EI31" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:180" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:180" s="5" customFormat="1" ht="15.5">
       <c r="A32" s="17" t="s">
         <v>389</v>
       </c>
@@ -11483,6 +11501,9 @@
       <c r="D32" s="18">
         <v>58</v>
       </c>
+      <c r="R32" s="5">
+        <v>1</v>
+      </c>
       <c r="BN32" t="s">
         <v>31</v>
       </c>
@@ -11495,27 +11516,66 @@
       <c r="BZ32" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="CB32" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="CD32" t="s">
         <v>32</v>
       </c>
+      <c r="CF32" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="CI32" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="CJ32" s="5">
+        <v>1</v>
+      </c>
+      <c r="CK32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DF32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DG32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DH32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DI32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DJ32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DK32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DL32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DN32" s="5">
+        <v>1</v>
+      </c>
+      <c r="DP32" s="5">
+        <v>1</v>
+      </c>
       <c r="EI32" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:180" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:180" s="5" customFormat="1">
       <c r="A33" s="17" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="34" spans="1:180" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:180" s="5" customFormat="1">
       <c r="A34" s="17" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="35" spans="1:180" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:180" s="5" customFormat="1">
       <c r="A35" s="17" t="s">
         <v>392</v>
       </c>
@@ -11523,50 +11583,50 @@
       <c r="FW35" s="6"/>
       <c r="FX35" s="7"/>
     </row>
-    <row r="36" spans="1:180" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:180" s="5" customFormat="1">
       <c r="A36" s="17" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="37" spans="1:180" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:180" s="5" customFormat="1">
       <c r="A37" s="17" t="s">
         <v>394</v>
       </c>
       <c r="EH37" s="6"/>
       <c r="EI37" s="7"/>
     </row>
-    <row r="38" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:180" s="5" customFormat="1"/>
+    <row r="39" spans="1:180" s="5" customFormat="1">
       <c r="EH39" s="6"/>
       <c r="EI39" s="7"/>
     </row>
-    <row r="40" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:180" s="5" customFormat="1">
       <c r="EH40" s="6"/>
       <c r="EI40" s="7"/>
     </row>
-    <row r="41" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:180" s="5" customFormat="1"/>
+    <row r="42" spans="1:180" s="5" customFormat="1">
       <c r="EH42" s="6"/>
       <c r="EI42" s="7"/>
     </row>
-    <row r="43" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:180" s="5" customFormat="1"/>
+    <row r="44" spans="1:180" s="5" customFormat="1">
       <c r="EH44" s="6"/>
       <c r="EI44" s="7"/>
     </row>
-    <row r="45" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:180" s="5" customFormat="1"/>
+    <row r="46" spans="1:180" s="5" customFormat="1"/>
+    <row r="47" spans="1:180" s="5" customFormat="1">
       <c r="EH47" s="6"/>
       <c r="EI47" s="7"/>
     </row>
-    <row r="48" spans="1:180" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:180" s="5" customFormat="1">
       <c r="EH48" s="6"/>
       <c r="EI48" s="7"/>
     </row>
-    <row r="49" spans="69:78" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="69:78" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="69:78" x14ac:dyDescent="0.2">
+    <row r="49" spans="69:78" s="5" customFormat="1"/>
+    <row r="50" spans="69:78" s="5" customFormat="1"/>
+    <row r="51" spans="69:78">
       <c r="BQ51" s="5"/>
       <c r="BR51" s="5"/>
       <c r="BS51" s="5"/>
@@ -11578,7 +11638,7 @@
       <c r="BY51" s="5"/>
       <c r="BZ51" s="5"/>
     </row>
-    <row r="52" spans="69:78" x14ac:dyDescent="0.2">
+    <row r="52" spans="69:78">
       <c r="BQ52" s="5"/>
       <c r="BR52" s="5"/>
       <c r="BS52" s="5"/>
@@ -11590,7 +11650,7 @@
       <c r="BY52" s="5"/>
       <c r="BZ52" s="5"/>
     </row>
-    <row r="53" spans="69:78" x14ac:dyDescent="0.2">
+    <row r="53" spans="69:78">
       <c r="BQ53" s="5"/>
       <c r="BR53" s="5"/>
       <c r="BS53" s="5"/>
@@ -11602,7 +11662,7 @@
       <c r="BY53" s="5"/>
       <c r="BZ53" s="5"/>
     </row>
-    <row r="54" spans="69:78" x14ac:dyDescent="0.2">
+    <row r="54" spans="69:78">
       <c r="BQ54" s="5"/>
       <c r="BR54" s="5"/>
       <c r="BS54" s="5"/>
@@ -11614,23 +11674,23 @@
       <c r="BY54" s="5"/>
       <c r="BZ54" s="5"/>
     </row>
-    <row r="72" spans="86:87" x14ac:dyDescent="0.2">
+    <row r="72" spans="86:87">
       <c r="CH72" s="1"/>
       <c r="CI72" s="2"/>
     </row>
-    <row r="73" spans="86:87" x14ac:dyDescent="0.2">
+    <row r="73" spans="86:87">
       <c r="CH73" s="1"/>
       <c r="CI73" s="2"/>
     </row>
-    <row r="74" spans="86:87" x14ac:dyDescent="0.2">
+    <row r="74" spans="86:87">
       <c r="CH74" s="1"/>
       <c r="CI74" s="2"/>
     </row>
-    <row r="75" spans="86:87" x14ac:dyDescent="0.2">
+    <row r="75" spans="86:87">
       <c r="CH75" s="1"/>
       <c r="CI75" s="2"/>
     </row>
-    <row r="76" spans="86:87" x14ac:dyDescent="0.2">
+    <row r="76" spans="86:87">
       <c r="CH76" s="1"/>
       <c r="CI76" s="2"/>
     </row>
@@ -11640,5 +11700,6 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>